<commit_message>
added paragrah analyzing Fig 4
</commit_message>
<xml_diff>
--- a/data/site-groups.xlsx
+++ b/data/site-groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiecooper/Independent Research Study/SignBase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF7E28D-9A6D-174B-9B2E-AC244CA1D4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EC3AD1-BAFA-4440-A0C8-CCF15D7E1FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{1013D442-849F-B941-B398-7419F84D3950}"/>
+    <workbookView xWindow="14520" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{1013D442-849F-B941-B398-7419F84D3950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,27 +50,12 @@
     <t>Geissenklösterle, Grotte du Renne, Vogelherd, Spy, La Ferrassie, Les Cottés</t>
   </si>
   <si>
-    <t>Hohle Fels, Solutré, Castanet, Cellier, Blanchard</t>
-  </si>
-  <si>
-    <t>Les Rois, Gargas, La Viña, Sirgenstein Cave</t>
-  </si>
-  <si>
     <t>Bockstein-Törle, Vogelherd,  Hohle Fels, Trou Magrite</t>
   </si>
   <si>
-    <t>Pod Hradem, Fumane,  Labeko Koba</t>
-  </si>
-  <si>
-    <t>El Castillo, Hohle Fels, Geissenklösterle</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Gatzarria, Hohlenstein-Stadel, Mladeč, Abri Pataud, </t>
   </si>
   <si>
-    <t>Grottes de Fonds-de-Forêt, Riparo Bombrini, Grotte de la Verpillière I, Vindija Cave, Trou al'Wesse</t>
-  </si>
-  <si>
     <t>Transitional</t>
   </si>
   <si>
@@ -81,6 +66,21 @@
   </si>
   <si>
     <t>Evolved Aurignacian</t>
+  </si>
+  <si>
+    <t>Pod Hradem, Fumane, Geissenklösterle</t>
+  </si>
+  <si>
+    <t>El Castillo, Hohle Fels, Labeko Koba</t>
+  </si>
+  <si>
+    <t>Hohle Fels, Solutré, Castanet, Cellier, Blanchard, Trou al'Wesse</t>
+  </si>
+  <si>
+    <t>Les Rois, Gargas, La Viña, Sirgenstein Cave,  Vindija Cave</t>
+  </si>
+  <si>
+    <t>Grottes de Fonds-de-Forêt, Riparo Bombrini, Grotte de la Verpillière I</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,40 +480,40 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -524,46 +524,46 @@
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>